<commit_message>
List of Scholars and Partner Schools
</commit_message>
<xml_diff>
--- a/Documents/SMFI Allowance file format.xlsx
+++ b/Documents/SMFI Allowance file format.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elly.bala\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Documents\SMF\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,24 +632,24 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -663,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -678,7 +678,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -693,7 +693,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -708,7 +708,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -723,12 +723,12 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -744,12 +744,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>100040001</v>
       </c>
@@ -777,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>100000102</v>
       </c>
@@ -791,7 +791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>100030109</v>
       </c>
@@ -805,7 +805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>100040802</v>
       </c>
@@ -819,7 +819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -837,7 +837,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -848,7 +848,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -859,7 +859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -870,7 +870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -883,6 +883,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>